<commit_message>
updated homework 1 and associated data files
</commit_message>
<xml_diff>
--- a/modules/data/Skykomish_peak_flow_12134500_skykomish_river_near_gold_bar.xlsx
+++ b/modules/data/Skykomish_peak_flow_12134500_skykomish_river_near_gold_bar.xlsx
@@ -1,16 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdlund/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D4BCD6-0367-A844-B958-B690D5E7A86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="1000" windowWidth="25040" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="11240" yWindow="600" windowWidth="25040" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="peak_flow_12134500_skykomish_ri" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -76,6 +91,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,19 +423,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10510</v>
       </c>
@@ -440,7 +463,7 @@
         <v>10.55</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>10994</v>
       </c>
@@ -455,7 +478,7 @@
         <v>10.44</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>11351</v>
       </c>
@@ -470,7 +493,7 @@
         <v>14.08</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>11745</v>
       </c>
@@ -485,7 +508,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>12006</v>
       </c>
@@ -500,7 +523,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>12409</v>
       </c>
@@ -515,7 +538,7 @@
         <v>21.28</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>12716</v>
       </c>
@@ -530,7 +553,7 @@
         <v>18.28</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>13286</v>
       </c>
@@ -545,7 +568,7 @@
         <v>10.91</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>13502</v>
       </c>
@@ -560,7 +583,7 @@
         <v>12.19</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>13988</v>
       </c>
@@ -575,7 +598,7 @@
         <v>16.37</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>14246</v>
       </c>
@@ -590,7 +613,7 @@
         <v>12.92</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>14594</v>
       </c>
@@ -602,7 +625,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>14943</v>
       </c>
@@ -617,7 +640,7 @@
         <v>11.38</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>15312</v>
       </c>
@@ -632,7 +655,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15668</v>
       </c>
@@ -647,7 +670,7 @@
         <v>14.08</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16043</v>
       </c>
@@ -662,7 +685,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16444</v>
       </c>
@@ -677,7 +700,7 @@
         <v>16.43</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>16735</v>
       </c>
@@ -692,7 +715,7 @@
         <v>13.95</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>17147</v>
       </c>
@@ -707,7 +730,7 @@
         <v>14.86</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>17459</v>
       </c>
@@ -722,7 +745,7 @@
         <v>15.67</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>17860</v>
       </c>
@@ -737,7 +760,7 @@
         <v>11.66</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>18229</v>
       </c>
@@ -752,7 +775,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>18669</v>
       </c>
@@ -767,7 +790,7 @@
         <v>18.87</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>18904</v>
       </c>
@@ -782,7 +805,7 @@
         <v>9.58</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>19390</v>
       </c>
@@ -797,7 +820,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>19702</v>
       </c>
@@ -812,7 +835,7 @@
         <v>12.84</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>20128</v>
       </c>
@@ -827,7 +850,7 @@
         <v>13.45</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>20434</v>
       </c>
@@ -842,7 +865,7 @@
         <v>16.13</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>20799</v>
       </c>
@@ -857,7 +880,7 @@
         <v>17.87</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>21202</v>
       </c>
@@ -872,7 +895,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>21501</v>
       </c>
@@ -887,7 +910,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>21877</v>
       </c>
@@ -902,7 +925,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>22296</v>
       </c>
@@ -917,7 +940,7 @@
         <v>15.11</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>22649</v>
       </c>
@@ -932,7 +955,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>22970</v>
       </c>
@@ -947,7 +970,7 @@
         <v>19.45</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>23377</v>
       </c>
@@ -962,7 +985,7 @@
         <v>12.21</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>23711</v>
       </c>
@@ -977,7 +1000,7 @@
         <v>13.41</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>24233</v>
       </c>
@@ -992,7 +1015,7 @@
         <v>11.07</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>24454</v>
       </c>
@@ -1007,7 +1030,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>24857</v>
       </c>
@@ -1022,7 +1045,7 @@
         <v>16.46</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>25208</v>
       </c>
@@ -1037,7 +1060,7 @@
         <v>15.36</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>25722</v>
       </c>
@@ -1052,7 +1075,7 @@
         <v>10.52</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>25952</v>
       </c>
@@ -1067,7 +1090,7 @@
         <v>14.06</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>26357</v>
       </c>
@@ -1082,7 +1105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>26659</v>
       </c>
@@ -1097,7 +1120,7 @@
         <v>14.61</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>27044</v>
       </c>
@@ -1112,7 +1135,7 @@
         <v>16.11</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>27384</v>
       </c>
@@ -1127,7 +1150,7 @@
         <v>15.48</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>27731</v>
       </c>
@@ -1142,7 +1165,7 @@
         <v>19.850000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>28143</v>
       </c>
@@ -1157,7 +1180,7 @@
         <v>14.17</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>28461</v>
       </c>
@@ -1172,7 +1195,7 @@
         <v>18.22</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>28798</v>
       </c>
@@ -1187,7 +1210,7 @@
         <v>12.28</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>29207</v>
       </c>
@@ -1202,7 +1225,7 @@
         <v>16.89</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>29581</v>
       </c>
@@ -1217,7 +1240,7 @@
         <v>21.34</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>29975</v>
       </c>
@@ -1232,7 +1255,7 @@
         <v>15.11</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>30288</v>
       </c>
@@ -1247,7 +1270,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>30685</v>
       </c>
@@ -1262,7 +1285,7 @@
         <v>15.18</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>31205</v>
       </c>
@@ -1277,7 +1300,7 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>31467</v>
       </c>
@@ -1292,7 +1315,7 @@
         <v>16.23</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>31739</v>
       </c>
@@ -1307,7 +1330,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>32120</v>
       </c>
@@ -1322,7 +1345,7 @@
         <v>14.43</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>32432</v>
       </c>
@@ -1337,7 +1360,7 @@
         <v>17.47</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>32846</v>
       </c>
@@ -1352,7 +1375,7 @@
         <v>17.440000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>33201</v>
       </c>
@@ -1367,7 +1390,7 @@
         <v>22.49</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>33577</v>
       </c>
@@ -1382,7 +1405,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>33994</v>
       </c>
@@ -1397,7 +1420,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>34395</v>
       </c>
@@ -1412,7 +1435,7 @@
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>34749</v>
       </c>
@@ -1427,7 +1450,7 @@
         <v>15.54</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>35032</v>
       </c>
@@ -1442,7 +1465,7 @@
         <v>20.239999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>35508</v>
       </c>
@@ -1457,7 +1480,7 @@
         <v>16.18</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>35733</v>
       </c>
@@ -1472,7 +1495,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>36158</v>
       </c>
@@ -1487,7 +1510,7 @@
         <v>18.72</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>36509</v>
       </c>
@@ -1502,7 +1525,7 @@
         <v>15.88</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>36800</v>
       </c>
@@ -1517,7 +1540,7 @@
         <v>11.05</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>37264</v>
       </c>
@@ -1532,7 +1555,7 @@
         <v>16.37</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>37647</v>
       </c>
@@ -1547,7 +1570,7 @@
         <v>16.38</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>37914</v>
       </c>
@@ -1562,7 +1585,7 @@
         <v>20.73</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>38370</v>
       </c>
@@ -1577,7 +1600,7 @@
         <v>19.55</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>38710</v>
       </c>
@@ -1592,7 +1615,7 @@
         <v>14.27</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>39027</v>
       </c>
@@ -1607,7 +1630,7 @@
         <v>24.51</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>39419</v>
       </c>
@@ -1622,7 +1645,7 @@
         <v>16.79</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>39821</v>
       </c>
@@ -1635,6 +1658,146 @@
       </c>
       <c r="D82">
         <v>19.48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>40560</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C83">
+        <v>63900</v>
+      </c>
+      <c r="D83">
+        <v>18.36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>40905</v>
+      </c>
+      <c r="B84" s="2">
+        <v>2012</v>
+      </c>
+      <c r="C84">
+        <v>25300</v>
+      </c>
+      <c r="D84">
+        <v>12.76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>41211</v>
+      </c>
+      <c r="B85" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C85">
+        <v>26800</v>
+      </c>
+      <c r="D85">
+        <v>13.05</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>41707</v>
+      </c>
+      <c r="B86" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C86">
+        <v>38900</v>
+      </c>
+      <c r="D86">
+        <v>15.08</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>41971</v>
+      </c>
+      <c r="B87" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C87">
+        <v>58100</v>
+      </c>
+      <c r="D87">
+        <v>17.670000000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>42325</v>
+      </c>
+      <c r="B88" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C88">
+        <v>95900</v>
+      </c>
+      <c r="D88">
+        <v>21.73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>42663</v>
+      </c>
+      <c r="B89" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C89">
+        <v>41000</v>
+      </c>
+      <c r="D89">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>43062</v>
+      </c>
+      <c r="B90" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C90">
+        <v>54200</v>
+      </c>
+      <c r="D90">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>43406</v>
+      </c>
+      <c r="B91" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C91">
+        <v>35200</v>
+      </c>
+      <c r="D91">
+        <v>14.98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B92" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C92">
+        <v>72200</v>
+      </c>
+      <c r="D92">
+        <v>19.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>